<commit_message>
add: uppdated data and code
</commit_message>
<xml_diff>
--- a/data/kidr_activity.xlsx
+++ b/data/kidr_activity.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\leobe\VSC1\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5C33B058-04B1-4C1E-9A65-D017D96DE870}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{496D7132-0904-41BF-8BAC-243DB38AF735}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="10470" yWindow="1480" windowWidth="8780" windowHeight="7960" xr2:uid="{E7A1553A-E805-9A4F-9906-A3E3D3A8C9B8}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{E7A1553A-E805-9A4F-9906-A3E3D3A8C9B8}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1 (3)" sheetId="5" r:id="rId1"/>
@@ -39,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="562" uniqueCount="233">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="563" uniqueCount="234">
   <si>
     <t>2020-178</t>
   </si>
@@ -738,6 +738,9 @@
   </si>
   <si>
     <t>2024-464</t>
+  </si>
+  <si>
+    <t>Visits</t>
   </si>
 </sst>
 </file>
@@ -809,7 +812,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="11">
+  <cellXfs count="15">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -831,6 +834,12 @@
       <alignment vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlänk" xfId="1" builtinId="8"/>
@@ -1166,10 +1175,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CB0C4C9A-925B-4803-AD4C-66BE80574A60}">
-  <dimension ref="A1:I65"/>
+  <dimension ref="A1:J65"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="60" zoomScaleNormal="60" workbookViewId="0">
-      <selection activeCell="A57" sqref="A57"/>
+    <sheetView tabSelected="1" topLeftCell="A8" zoomScale="60" zoomScaleNormal="60" workbookViewId="0">
+      <selection activeCell="E55" sqref="E55"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10.6640625" defaultRowHeight="16" x14ac:dyDescent="0.4"/>
@@ -1178,51 +1187,55 @@
     <col min="2" max="2" width="26" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="22.33203125" customWidth="1"/>
     <col min="4" max="4" width="25.4140625" customWidth="1"/>
-    <col min="5" max="5" width="24.58203125" customWidth="1"/>
-    <col min="6" max="6" width="26.33203125" customWidth="1"/>
-    <col min="7" max="7" width="34.5" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="27.5" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="40" customWidth="1"/>
+    <col min="5" max="5" width="25.4140625" style="13" customWidth="1"/>
+    <col min="6" max="6" width="24.58203125" customWidth="1"/>
+    <col min="7" max="7" width="26.33203125" customWidth="1"/>
+    <col min="8" max="8" width="34.5" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="27.5" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="40" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" ht="31" x14ac:dyDescent="0.7">
+    <row r="1" spans="1:10" ht="31" x14ac:dyDescent="0.7">
       <c r="A1" s="7" t="s">
         <v>90</v>
       </c>
       <c r="B1" s="7"/>
       <c r="C1" s="7"/>
       <c r="D1" s="7"/>
-      <c r="E1" s="7"/>
+      <c r="E1" s="11"/>
       <c r="F1" s="7"/>
       <c r="G1" s="7"/>
       <c r="H1" s="7"/>
       <c r="I1" s="7"/>
-    </row>
-    <row r="2" spans="1:9" ht="31" x14ac:dyDescent="0.7">
+      <c r="J1" s="7"/>
+    </row>
+    <row r="2" spans="1:10" ht="31" x14ac:dyDescent="0.7">
       <c r="A2" s="7" t="s">
         <v>91</v>
       </c>
       <c r="B2" s="7"/>
       <c r="C2" s="7"/>
       <c r="D2" s="7"/>
-      <c r="E2" s="7"/>
+      <c r="E2" s="11"/>
       <c r="F2" s="7"/>
       <c r="G2" s="7"/>
       <c r="H2" s="7"/>
       <c r="I2" s="7"/>
-    </row>
-    <row r="3" spans="1:9" ht="31" x14ac:dyDescent="0.7">
+      <c r="J2" s="7"/>
+    </row>
+    <row r="3" spans="1:10" ht="31" x14ac:dyDescent="0.7">
       <c r="A3" s="7"/>
       <c r="B3" s="7"/>
       <c r="C3" s="7"/>
       <c r="D3" s="7"/>
-      <c r="E3" s="7"/>
+      <c r="E3" s="11"/>
       <c r="F3" s="7"/>
       <c r="G3" s="7"/>
       <c r="H3" s="7"/>
       <c r="I3" s="7"/>
-    </row>
-    <row r="4" spans="1:9" ht="31" x14ac:dyDescent="0.7">
+      <c r="J3" s="7"/>
+    </row>
+    <row r="4" spans="1:10" ht="31" x14ac:dyDescent="0.7">
       <c r="A4" s="7" t="s">
         <v>85</v>
       </c>
@@ -1235,1081 +1248,1126 @@
       <c r="D4" s="7" t="s">
         <v>88</v>
       </c>
-      <c r="E4" s="7" t="s">
+      <c r="E4" s="11" t="s">
+        <v>233</v>
+      </c>
+      <c r="F4" s="7" t="s">
         <v>122</v>
       </c>
-      <c r="F4" s="7" t="s">
+      <c r="G4" s="7" t="s">
         <v>144</v>
       </c>
-      <c r="G4" s="7" t="s">
+      <c r="H4" s="7" t="s">
         <v>89</v>
       </c>
-      <c r="H4" s="7" t="s">
+      <c r="I4" s="7" t="s">
         <v>94</v>
       </c>
-      <c r="I4" s="8" t="s">
+      <c r="J4" s="8" t="s">
         <v>92</v>
       </c>
     </row>
-    <row r="5" spans="1:9" x14ac:dyDescent="0.4">
-      <c r="A5" s="1" t="s">
+    <row r="5" spans="1:10" x14ac:dyDescent="0.4">
+      <c r="A5" s="3" t="s">
+        <v>211</v>
+      </c>
+      <c r="B5" s="1">
+        <v>16</v>
+      </c>
+      <c r="C5" s="1" t="s">
+        <v>142</v>
+      </c>
+      <c r="D5" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="E5" s="12"/>
+      <c r="F5">
+        <v>1013</v>
+      </c>
+      <c r="G5" s="1"/>
+      <c r="H5" s="1"/>
+      <c r="I5" s="1"/>
+      <c r="J5" s="2"/>
+    </row>
+    <row r="6" spans="1:10" x14ac:dyDescent="0.4">
+      <c r="A6" t="s">
+        <v>230</v>
+      </c>
+      <c r="C6" t="s">
+        <v>206</v>
+      </c>
+      <c r="D6" s="10">
+        <v>44067</v>
+      </c>
+      <c r="E6" s="13">
+        <v>31</v>
+      </c>
+      <c r="F6">
+        <v>1294</v>
+      </c>
+    </row>
+    <row r="7" spans="1:10" x14ac:dyDescent="0.4">
+      <c r="A7" s="1" t="s">
         <v>210</v>
       </c>
-      <c r="B5" s="1">
+      <c r="B7" s="1">
         <v>70757</v>
       </c>
-      <c r="C5" s="1">
+      <c r="C7" s="1">
         <v>1100000</v>
       </c>
-      <c r="D5" s="1" t="s">
+      <c r="D7" s="1" t="s">
         <v>84</v>
       </c>
-      <c r="E5">
+      <c r="E7" s="12">
+        <v>178</v>
+      </c>
+      <c r="F7">
         <v>1062</v>
       </c>
-      <c r="F5" s="1">
+      <c r="G7" s="1">
         <v>1</v>
       </c>
-      <c r="G5" s="1">
-        <v>2</v>
-      </c>
-      <c r="H5" s="1">
+      <c r="H7" s="1">
+        <v>2</v>
+      </c>
+      <c r="I7" s="1">
         <v>0</v>
       </c>
-      <c r="I5" s="2" t="s">
+      <c r="J7" s="2" t="s">
         <v>145</v>
       </c>
     </row>
-    <row r="6" spans="1:9" x14ac:dyDescent="0.4">
-      <c r="A6" s="3" t="s">
-        <v>211</v>
-      </c>
-      <c r="B6" s="1">
-        <v>16</v>
-      </c>
-      <c r="C6" s="1" t="s">
-        <v>142</v>
-      </c>
-      <c r="D6" s="1" t="s">
+    <row r="8" spans="1:10" x14ac:dyDescent="0.4">
+      <c r="A8" t="s">
+        <v>229</v>
+      </c>
+      <c r="C8" t="s">
+        <v>209</v>
+      </c>
+      <c r="D8" s="10">
+        <v>44371</v>
+      </c>
+      <c r="E8" s="13">
+        <v>26</v>
+      </c>
+      <c r="F8">
+        <v>1355</v>
+      </c>
+    </row>
+    <row r="9" spans="1:10" x14ac:dyDescent="0.4">
+      <c r="A9" s="3" t="s">
+        <v>212</v>
+      </c>
+      <c r="B9" s="1">
+        <v>23</v>
+      </c>
+      <c r="C9" s="1" t="s">
+        <v>143</v>
+      </c>
+      <c r="D9" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="E9" s="12">
+        <v>77</v>
+      </c>
+      <c r="F9">
+        <v>1012</v>
+      </c>
+      <c r="G9" s="1">
+        <v>2</v>
+      </c>
+      <c r="H9" s="1">
+        <v>4</v>
+      </c>
+      <c r="I9" s="1">
         <v>1</v>
       </c>
-      <c r="E6">
-        <v>1013</v>
-      </c>
-      <c r="F6" s="1"/>
-      <c r="G6" s="1"/>
-      <c r="H6" s="1"/>
-      <c r="I6" s="2"/>
-    </row>
-    <row r="7" spans="1:9" x14ac:dyDescent="0.4">
-      <c r="A7" s="3" t="s">
-        <v>212</v>
-      </c>
-      <c r="B7" s="1">
-        <v>23</v>
-      </c>
-      <c r="C7" s="1" t="s">
-        <v>143</v>
-      </c>
-      <c r="D7" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="E7">
+      <c r="J9" s="2"/>
+    </row>
+    <row r="10" spans="1:10" ht="108.5" x14ac:dyDescent="0.4">
+      <c r="A10" s="4" t="s">
+        <v>213</v>
+      </c>
+      <c r="B10" s="5">
+        <v>99796</v>
+      </c>
+      <c r="C10" s="5">
+        <v>2300000</v>
+      </c>
+      <c r="D10" s="5" t="s">
+        <v>83</v>
+      </c>
+      <c r="E10" s="14">
+        <v>3191</v>
+      </c>
+      <c r="F10">
+        <v>1062</v>
+      </c>
+      <c r="G10" s="5">
+        <v>1</v>
+      </c>
+      <c r="H10" s="5">
+        <v>150</v>
+      </c>
+      <c r="I10" s="5">
+        <v>146</v>
+      </c>
+      <c r="J10" s="2" t="s">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="11" spans="1:10" x14ac:dyDescent="0.4">
+      <c r="A11" s="3" t="s">
+        <v>214</v>
+      </c>
+      <c r="B11" s="1">
+        <v>11</v>
+      </c>
+      <c r="C11" s="1" t="s">
+        <v>123</v>
+      </c>
+      <c r="D11" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="E11" s="12">
+        <v>22</v>
+      </c>
+      <c r="F11">
+        <v>367</v>
+      </c>
+      <c r="G11" s="1"/>
+      <c r="H11" s="1">
+        <v>2</v>
+      </c>
+      <c r="I11" s="1">
+        <v>2</v>
+      </c>
+      <c r="J11" s="2"/>
+    </row>
+    <row r="12" spans="1:10" x14ac:dyDescent="0.4">
+      <c r="A12" s="3" t="s">
+        <v>215</v>
+      </c>
+      <c r="B12" s="1">
+        <v>10</v>
+      </c>
+      <c r="C12" s="1" t="s">
+        <v>124</v>
+      </c>
+      <c r="D12" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="E12" s="12"/>
+      <c r="F12">
+        <v>367</v>
+      </c>
+      <c r="G12" s="1"/>
+      <c r="H12" s="1">
+        <v>2</v>
+      </c>
+      <c r="I12" s="1">
+        <v>2</v>
+      </c>
+      <c r="J12" s="2"/>
+    </row>
+    <row r="13" spans="1:10" x14ac:dyDescent="0.4">
+      <c r="A13" s="3" t="s">
+        <v>216</v>
+      </c>
+      <c r="B13" s="1">
+        <v>17</v>
+      </c>
+      <c r="C13" s="1" t="s">
+        <v>125</v>
+      </c>
+      <c r="D13" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="E13" s="12">
+        <v>13</v>
+      </c>
+      <c r="F13">
         <v>1012</v>
       </c>
-      <c r="F7" s="1">
-        <v>2</v>
-      </c>
-      <c r="G7" s="1">
-        <v>4</v>
-      </c>
-      <c r="H7" s="1">
-        <v>1</v>
-      </c>
-      <c r="I7" s="2"/>
-    </row>
-    <row r="8" spans="1:9" ht="108.5" x14ac:dyDescent="0.4">
-      <c r="A8" s="4" t="s">
-        <v>213</v>
-      </c>
-      <c r="B8" s="5">
-        <v>99796</v>
-      </c>
-      <c r="C8" s="5">
-        <v>2300000</v>
-      </c>
-      <c r="D8" s="5" t="s">
-        <v>83</v>
-      </c>
-      <c r="E8">
-        <v>1062</v>
-      </c>
-      <c r="F8" s="5">
-        <v>1</v>
-      </c>
-      <c r="G8" s="5">
-        <v>150</v>
-      </c>
-      <c r="H8" s="5">
-        <v>146</v>
-      </c>
-      <c r="I8" s="2" t="s">
-        <v>93</v>
-      </c>
-    </row>
-    <row r="9" spans="1:9" x14ac:dyDescent="0.4">
-      <c r="A9" s="3" t="s">
-        <v>214</v>
-      </c>
-      <c r="B9" s="1">
-        <v>11</v>
-      </c>
-      <c r="C9" s="1" t="s">
-        <v>123</v>
-      </c>
-      <c r="D9" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="E9">
-        <v>367</v>
-      </c>
-      <c r="F9" s="1"/>
-      <c r="G9" s="1">
-        <v>2</v>
-      </c>
-      <c r="H9" s="1">
-        <v>2</v>
-      </c>
-      <c r="I9" s="2"/>
-    </row>
-    <row r="10" spans="1:9" x14ac:dyDescent="0.4">
-      <c r="A10" s="3" t="s">
-        <v>215</v>
-      </c>
-      <c r="B10" s="1">
-        <v>10</v>
-      </c>
-      <c r="C10" s="1" t="s">
-        <v>124</v>
-      </c>
-      <c r="D10" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="E10">
-        <v>367</v>
-      </c>
-      <c r="F10" s="1"/>
-      <c r="G10" s="1">
-        <v>2</v>
-      </c>
-      <c r="H10" s="1">
-        <v>2</v>
-      </c>
-      <c r="I10" s="2"/>
-    </row>
-    <row r="11" spans="1:9" x14ac:dyDescent="0.4">
-      <c r="A11" s="3" t="s">
-        <v>216</v>
-      </c>
-      <c r="B11" s="1">
-        <v>17</v>
-      </c>
-      <c r="C11" s="1" t="s">
-        <v>125</v>
-      </c>
-      <c r="D11" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="E11">
-        <v>1012</v>
-      </c>
-      <c r="F11" s="1"/>
-      <c r="G11" s="1"/>
-      <c r="H11" s="1"/>
-      <c r="I11" s="2"/>
-    </row>
-    <row r="12" spans="1:9" x14ac:dyDescent="0.4">
-      <c r="A12" s="3" t="s">
-        <v>217</v>
-      </c>
-      <c r="B12" s="1">
-        <v>17</v>
-      </c>
-      <c r="C12" s="1" t="s">
-        <v>126</v>
-      </c>
-      <c r="D12" s="1" t="s">
-        <v>16</v>
-      </c>
-      <c r="E12">
-        <v>1012</v>
-      </c>
-      <c r="F12" s="1">
-        <v>0</v>
-      </c>
-      <c r="G12" s="1">
-        <v>1</v>
-      </c>
-      <c r="H12" s="1">
-        <v>0</v>
-      </c>
-      <c r="I12" s="1"/>
-    </row>
-    <row r="13" spans="1:9" x14ac:dyDescent="0.4">
-      <c r="A13" s="3" t="s">
-        <v>218</v>
-      </c>
-      <c r="B13" s="1">
-        <v>15</v>
-      </c>
-      <c r="C13" s="1" t="s">
-        <v>127</v>
-      </c>
-      <c r="D13" s="1" t="s">
-        <v>18</v>
-      </c>
-      <c r="E13">
-        <v>1013</v>
-      </c>
-      <c r="F13" s="1"/>
       <c r="G13" s="1"/>
       <c r="H13" s="1"/>
       <c r="I13" s="1"/>
-    </row>
-    <row r="14" spans="1:9" x14ac:dyDescent="0.4">
+      <c r="J13" s="2"/>
+    </row>
+    <row r="14" spans="1:10" x14ac:dyDescent="0.4">
       <c r="A14" s="3" t="s">
-        <v>219</v>
+        <v>217</v>
       </c>
       <c r="B14" s="1">
-        <v>150</v>
-      </c>
-      <c r="C14" s="1">
-        <v>255450</v>
+        <v>17</v>
+      </c>
+      <c r="C14" s="1" t="s">
+        <v>126</v>
       </c>
       <c r="D14" s="1" t="s">
-        <v>20</v>
-      </c>
-      <c r="E14">
-        <v>983</v>
-      </c>
-      <c r="F14" s="1"/>
-      <c r="G14" s="1"/>
-      <c r="H14" s="1"/>
-      <c r="I14" s="1"/>
-    </row>
-    <row r="15" spans="1:9" x14ac:dyDescent="0.4">
+        <v>16</v>
+      </c>
+      <c r="E14" s="12">
+        <v>11</v>
+      </c>
+      <c r="F14">
+        <v>1012</v>
+      </c>
+      <c r="G14" s="1">
+        <v>0</v>
+      </c>
+      <c r="H14" s="1">
+        <v>1</v>
+      </c>
+      <c r="I14" s="1">
+        <v>0</v>
+      </c>
+      <c r="J14" s="1"/>
+    </row>
+    <row r="15" spans="1:10" x14ac:dyDescent="0.4">
       <c r="A15" s="3" t="s">
-        <v>220</v>
+        <v>218</v>
       </c>
       <c r="B15" s="1">
-        <v>8</v>
+        <v>15</v>
       </c>
       <c r="C15" s="1" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="D15" s="1" t="s">
-        <v>22</v>
-      </c>
-      <c r="E15">
-        <v>657</v>
-      </c>
-      <c r="F15" s="1"/>
+        <v>18</v>
+      </c>
+      <c r="E15" s="12"/>
+      <c r="F15">
+        <v>1013</v>
+      </c>
       <c r="G15" s="1"/>
       <c r="H15" s="1"/>
       <c r="I15" s="1"/>
-    </row>
-    <row r="16" spans="1:9" x14ac:dyDescent="0.4">
-      <c r="A16" s="3" t="s">
+      <c r="J15" s="1"/>
+    </row>
+    <row r="16" spans="1:10" x14ac:dyDescent="0.4">
+      <c r="A16" t="s">
+        <v>228</v>
+      </c>
+      <c r="C16" t="s">
+        <v>205</v>
+      </c>
+      <c r="D16" s="10">
+        <v>44812</v>
+      </c>
+      <c r="E16" s="12">
+        <v>62</v>
+      </c>
+      <c r="F16">
+        <v>914</v>
+      </c>
+    </row>
+    <row r="17" spans="1:10" x14ac:dyDescent="0.4">
+      <c r="A17" s="3" t="s">
+        <v>219</v>
+      </c>
+      <c r="B17" s="1">
+        <v>150</v>
+      </c>
+      <c r="C17" s="1">
+        <v>255450</v>
+      </c>
+      <c r="D17" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="E17" s="12">
+        <v>14</v>
+      </c>
+      <c r="F17">
+        <v>983</v>
+      </c>
+      <c r="G17" s="1"/>
+      <c r="H17" s="1"/>
+      <c r="I17" s="1"/>
+      <c r="J17" s="1"/>
+    </row>
+    <row r="18" spans="1:10" x14ac:dyDescent="0.4">
+      <c r="A18" t="s">
+        <v>227</v>
+      </c>
+      <c r="C18" t="s">
+        <v>204</v>
+      </c>
+      <c r="D18" s="10">
+        <v>44928</v>
+      </c>
+      <c r="E18" s="12">
+        <v>3445</v>
+      </c>
+      <c r="F18">
+        <v>798</v>
+      </c>
+    </row>
+    <row r="19" spans="1:10" x14ac:dyDescent="0.4">
+      <c r="A19" s="3" t="s">
+        <v>220</v>
+      </c>
+      <c r="B19" s="1">
+        <v>8</v>
+      </c>
+      <c r="C19" s="1" t="s">
+        <v>128</v>
+      </c>
+      <c r="D19" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="E19" s="12">
+        <v>11</v>
+      </c>
+      <c r="F19">
+        <v>657</v>
+      </c>
+      <c r="G19" s="1"/>
+      <c r="H19" s="1"/>
+      <c r="I19" s="1"/>
+      <c r="J19" s="1"/>
+    </row>
+    <row r="20" spans="1:10" x14ac:dyDescent="0.4">
+      <c r="A20" t="s">
+        <v>226</v>
+      </c>
+      <c r="C20" t="s">
+        <v>202</v>
+      </c>
+      <c r="D20" s="10">
+        <v>45069</v>
+      </c>
+      <c r="F20">
+        <v>657</v>
+      </c>
+    </row>
+    <row r="21" spans="1:10" x14ac:dyDescent="0.4">
+      <c r="A21" s="3" t="s">
         <v>221</v>
       </c>
-      <c r="B16" s="1">
+      <c r="B21" s="1">
         <v>23</v>
       </c>
-      <c r="C16" s="1">
+      <c r="C21" s="1">
         <v>8250</v>
       </c>
-      <c r="D16" s="1" t="s">
+      <c r="D21" s="1" t="s">
         <v>24</v>
       </c>
-      <c r="E16">
+      <c r="E21" s="12">
+        <v>12</v>
+      </c>
+      <c r="F21">
         <v>649</v>
       </c>
-      <c r="F16" s="1"/>
-      <c r="G16" s="1"/>
-      <c r="H16" s="1"/>
-      <c r="I16" s="1"/>
-    </row>
-    <row r="17" spans="1:9" x14ac:dyDescent="0.4">
-      <c r="A17" s="3" t="s">
-        <v>222</v>
-      </c>
-      <c r="B17" s="1">
-        <v>91</v>
-      </c>
-      <c r="C17" s="1">
-        <v>361450</v>
-      </c>
-      <c r="D17" s="1" t="s">
-        <v>26</v>
-      </c>
-      <c r="E17">
-        <v>643</v>
-      </c>
-      <c r="F17" s="1">
-        <v>1</v>
-      </c>
-      <c r="G17" s="1">
-        <v>2</v>
-      </c>
-      <c r="H17" s="1">
-        <v>1</v>
-      </c>
-      <c r="I17" s="1"/>
-    </row>
-    <row r="18" spans="1:9" x14ac:dyDescent="0.4">
-      <c r="A18" s="3" t="s">
-        <v>223</v>
-      </c>
-      <c r="B18" s="1">
-        <v>93</v>
-      </c>
-      <c r="C18" s="1">
-        <v>209850</v>
-      </c>
-      <c r="D18" s="1" t="s">
-        <v>28</v>
-      </c>
-      <c r="E18">
-        <v>642</v>
-      </c>
-      <c r="F18" s="1">
-        <v>1</v>
-      </c>
-      <c r="G18" s="1">
-        <v>5</v>
-      </c>
-      <c r="H18" s="1">
-        <v>3</v>
-      </c>
-      <c r="I18" s="1"/>
-    </row>
-    <row r="19" spans="1:9" x14ac:dyDescent="0.4">
-      <c r="A19" s="3" t="s">
-        <v>224</v>
-      </c>
-      <c r="B19" s="1">
-        <v>27</v>
-      </c>
-      <c r="C19" s="1">
-        <v>305910</v>
-      </c>
-      <c r="D19" s="1" t="s">
-        <v>30</v>
-      </c>
-      <c r="E19">
-        <v>636</v>
-      </c>
-      <c r="F19" s="1">
-        <v>1</v>
-      </c>
-      <c r="G19" s="1">
-        <v>3</v>
-      </c>
-      <c r="H19" s="1">
-        <v>2</v>
-      </c>
-      <c r="I19" s="1"/>
-    </row>
-    <row r="20" spans="1:9" x14ac:dyDescent="0.4">
-      <c r="A20" s="3" t="s">
-        <v>31</v>
-      </c>
-      <c r="B20" s="1">
-        <v>5</v>
-      </c>
-      <c r="C20" s="1">
-        <v>1330000</v>
-      </c>
-      <c r="D20" s="1" t="s">
-        <v>32</v>
-      </c>
-      <c r="E20">
-        <v>613</v>
-      </c>
-      <c r="F20" s="1"/>
-      <c r="G20" s="1"/>
-      <c r="H20" s="1"/>
-      <c r="I20" s="1"/>
-    </row>
-    <row r="21" spans="1:9" x14ac:dyDescent="0.4">
-      <c r="A21" s="3" t="s">
-        <v>33</v>
-      </c>
-      <c r="B21" s="1">
-        <v>16</v>
-      </c>
-      <c r="C21" s="1" t="s">
-        <v>129</v>
-      </c>
-      <c r="D21" s="1" t="s">
-        <v>34</v>
-      </c>
-      <c r="E21">
-        <v>529</v>
-      </c>
-      <c r="F21" s="1"/>
       <c r="G21" s="1"/>
       <c r="H21" s="1"/>
       <c r="I21" s="1"/>
-    </row>
-    <row r="22" spans="1:9" x14ac:dyDescent="0.4">
+      <c r="J21" s="1"/>
+    </row>
+    <row r="22" spans="1:10" x14ac:dyDescent="0.4">
       <c r="A22" s="3" t="s">
-        <v>35</v>
+        <v>222</v>
       </c>
       <c r="B22" s="1">
-        <v>53</v>
+        <v>91</v>
       </c>
       <c r="C22" s="1">
-        <v>4290</v>
+        <v>361450</v>
       </c>
       <c r="D22" s="1" t="s">
-        <v>36</v>
-      </c>
-      <c r="E22">
-        <v>469</v>
-      </c>
-      <c r="F22" s="1"/>
+        <v>26</v>
+      </c>
+      <c r="E22" s="12">
+        <v>187</v>
+      </c>
+      <c r="F22">
+        <v>643</v>
+      </c>
       <c r="G22" s="1">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="H22" s="1">
-        <v>0</v>
-      </c>
-      <c r="I22" s="1"/>
-    </row>
-    <row r="23" spans="1:9" x14ac:dyDescent="0.4">
+        <v>2</v>
+      </c>
+      <c r="I22" s="1">
+        <v>1</v>
+      </c>
+      <c r="J22" s="1"/>
+    </row>
+    <row r="23" spans="1:10" x14ac:dyDescent="0.4">
       <c r="A23" s="3" t="s">
-        <v>37</v>
+        <v>223</v>
       </c>
       <c r="B23" s="1">
-        <v>22</v>
+        <v>93</v>
       </c>
       <c r="C23" s="1">
-        <v>80910</v>
+        <v>209850</v>
       </c>
       <c r="D23" s="1" t="s">
-        <v>38</v>
-      </c>
-      <c r="E23">
-        <v>507</v>
-      </c>
-      <c r="F23" s="1"/>
-      <c r="G23" s="1"/>
-      <c r="H23" s="1"/>
-      <c r="I23" s="1"/>
-    </row>
-    <row r="24" spans="1:9" x14ac:dyDescent="0.4">
+        <v>28</v>
+      </c>
+      <c r="E23" s="12">
+        <v>149</v>
+      </c>
+      <c r="F23">
+        <v>642</v>
+      </c>
+      <c r="G23" s="1">
+        <v>1</v>
+      </c>
+      <c r="H23" s="1">
+        <v>5</v>
+      </c>
+      <c r="I23" s="1">
+        <v>3</v>
+      </c>
+      <c r="J23" s="1"/>
+    </row>
+    <row r="24" spans="1:10" x14ac:dyDescent="0.4">
       <c r="A24" s="3" t="s">
-        <v>39</v>
+        <v>224</v>
       </c>
       <c r="B24" s="1">
-        <v>41</v>
+        <v>27</v>
       </c>
       <c r="C24" s="1">
-        <v>187170</v>
+        <v>305910</v>
       </c>
       <c r="D24" s="1" t="s">
-        <v>40</v>
-      </c>
-      <c r="E24">
-        <v>504</v>
-      </c>
-      <c r="F24" s="1"/>
-      <c r="G24" s="1"/>
-      <c r="H24" s="1"/>
-      <c r="I24" s="1"/>
-    </row>
-    <row r="25" spans="1:9" x14ac:dyDescent="0.4">
+        <v>30</v>
+      </c>
+      <c r="E24" s="12">
+        <v>144</v>
+      </c>
+      <c r="F24">
+        <v>636</v>
+      </c>
+      <c r="G24" s="1">
+        <v>1</v>
+      </c>
+      <c r="H24" s="1">
+        <v>3</v>
+      </c>
+      <c r="I24" s="1">
+        <v>2</v>
+      </c>
+      <c r="J24" s="1"/>
+    </row>
+    <row r="25" spans="1:10" x14ac:dyDescent="0.4">
       <c r="A25" s="3" t="s">
-        <v>41</v>
+        <v>31</v>
       </c>
       <c r="B25" s="1">
-        <v>68</v>
+        <v>5</v>
       </c>
       <c r="C25" s="1">
-        <v>1840000</v>
+        <v>1330000</v>
       </c>
       <c r="D25" s="1" t="s">
-        <v>42</v>
-      </c>
-      <c r="E25">
-        <v>508</v>
-      </c>
-      <c r="F25" s="1"/>
+        <v>32</v>
+      </c>
+      <c r="E25" s="12">
+        <v>91</v>
+      </c>
+      <c r="F25">
+        <v>613</v>
+      </c>
       <c r="G25" s="1"/>
       <c r="H25" s="1"/>
       <c r="I25" s="1"/>
-    </row>
-    <row r="26" spans="1:9" x14ac:dyDescent="0.4">
+      <c r="J25" s="1"/>
+    </row>
+    <row r="26" spans="1:10" x14ac:dyDescent="0.4">
       <c r="A26" s="3" t="s">
-        <v>225</v>
+        <v>33</v>
       </c>
       <c r="B26" s="1">
         <v>16</v>
       </c>
       <c r="C26" s="1" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="D26" s="1" t="s">
-        <v>44</v>
-      </c>
-      <c r="E26">
-        <v>714</v>
-      </c>
-      <c r="F26" s="1">
-        <v>1</v>
-      </c>
-      <c r="G26" s="1">
-        <v>1</v>
-      </c>
-      <c r="H26" s="1">
+        <v>34</v>
+      </c>
+      <c r="E26" s="12">
+        <v>7</v>
+      </c>
+      <c r="F26">
+        <v>529</v>
+      </c>
+      <c r="G26" s="1"/>
+      <c r="H26" s="1"/>
+      <c r="I26" s="1"/>
+      <c r="J26" s="1"/>
+    </row>
+    <row r="27" spans="1:10" x14ac:dyDescent="0.4">
+      <c r="A27" s="3" t="s">
+        <v>35</v>
+      </c>
+      <c r="B27" s="1">
+        <v>53</v>
+      </c>
+      <c r="C27" s="1">
+        <v>4290</v>
+      </c>
+      <c r="D27" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="E27" s="12">
+        <v>157</v>
+      </c>
+      <c r="F27">
+        <v>469</v>
+      </c>
+      <c r="G27" s="1"/>
+      <c r="H27" s="1">
+        <v>2</v>
+      </c>
+      <c r="I27" s="1">
         <v>0</v>
       </c>
-      <c r="I26" s="1"/>
-    </row>
-    <row r="27" spans="1:9" x14ac:dyDescent="0.4">
-      <c r="A27" s="3" t="s">
-        <v>45</v>
-      </c>
-      <c r="B27" s="1">
-        <v>56</v>
-      </c>
-      <c r="C27" s="1">
-        <v>24590</v>
-      </c>
-      <c r="D27" s="1" t="s">
-        <v>46</v>
-      </c>
-      <c r="E27">
-        <v>454</v>
-      </c>
-      <c r="F27" s="1"/>
-      <c r="G27" s="1"/>
-      <c r="H27" s="1"/>
-      <c r="I27" s="1"/>
-    </row>
-    <row r="28" spans="1:9" x14ac:dyDescent="0.4">
+      <c r="J27" s="1"/>
+    </row>
+    <row r="28" spans="1:10" x14ac:dyDescent="0.4">
       <c r="A28" s="3" t="s">
-        <v>51</v>
+        <v>37</v>
       </c>
       <c r="B28" s="1">
-        <v>7</v>
-      </c>
-      <c r="C28" s="1" t="s">
-        <v>131</v>
+        <v>22</v>
+      </c>
+      <c r="C28" s="1">
+        <v>80910</v>
       </c>
       <c r="D28" s="1" t="s">
-        <v>53</v>
-      </c>
-      <c r="E28">
-        <v>199</v>
-      </c>
-      <c r="F28" s="1"/>
-      <c r="G28" s="1">
-        <v>4</v>
-      </c>
-      <c r="H28" s="1">
-        <v>4</v>
-      </c>
+        <v>38</v>
+      </c>
+      <c r="E28" s="12">
+        <v>10</v>
+      </c>
+      <c r="F28">
+        <v>507</v>
+      </c>
+      <c r="G28" s="1"/>
+      <c r="H28" s="1"/>
       <c r="I28" s="1"/>
-    </row>
-    <row r="29" spans="1:9" x14ac:dyDescent="0.4">
+      <c r="J28" s="1"/>
+    </row>
+    <row r="29" spans="1:10" x14ac:dyDescent="0.4">
       <c r="A29" s="3" t="s">
-        <v>54</v>
+        <v>39</v>
       </c>
       <c r="B29" s="1">
-        <v>6</v>
-      </c>
-      <c r="C29" s="1" t="s">
-        <v>132</v>
+        <v>41</v>
+      </c>
+      <c r="C29" s="1">
+        <v>187170</v>
       </c>
       <c r="D29" s="1" t="s">
-        <v>55</v>
-      </c>
-      <c r="E29">
-        <v>224</v>
-      </c>
-      <c r="F29" s="1"/>
-      <c r="G29" s="1">
-        <v>1</v>
-      </c>
-      <c r="H29" s="1">
-        <v>0</v>
-      </c>
+        <v>40</v>
+      </c>
+      <c r="E29" s="12">
+        <v>19</v>
+      </c>
+      <c r="F29">
+        <v>504</v>
+      </c>
+      <c r="G29" s="1"/>
+      <c r="H29" s="1"/>
       <c r="I29" s="1"/>
-    </row>
-    <row r="30" spans="1:9" x14ac:dyDescent="0.4">
+      <c r="J29" s="1"/>
+    </row>
+    <row r="30" spans="1:10" x14ac:dyDescent="0.4">
       <c r="A30" s="3" t="s">
-        <v>56</v>
+        <v>41</v>
       </c>
       <c r="B30" s="1">
-        <v>5</v>
-      </c>
-      <c r="C30" s="1" t="s">
-        <v>133</v>
+        <v>68</v>
+      </c>
+      <c r="C30" s="1">
+        <v>1840000</v>
       </c>
       <c r="D30" s="1" t="s">
-        <v>57</v>
-      </c>
-      <c r="E30">
-        <v>31</v>
-      </c>
-      <c r="F30" s="1"/>
+        <v>42</v>
+      </c>
+      <c r="E30" s="12">
+        <v>18</v>
+      </c>
+      <c r="F30">
+        <v>508</v>
+      </c>
       <c r="G30" s="1"/>
       <c r="H30" s="1"/>
       <c r="I30" s="1"/>
-    </row>
-    <row r="31" spans="1:9" x14ac:dyDescent="0.4">
+      <c r="J30" s="1"/>
+    </row>
+    <row r="31" spans="1:10" x14ac:dyDescent="0.4">
       <c r="A31" s="3" t="s">
-        <v>60</v>
+        <v>225</v>
       </c>
       <c r="B31" s="1">
-        <v>121</v>
+        <v>16</v>
       </c>
       <c r="C31" s="1" t="s">
-        <v>134</v>
+        <v>130</v>
       </c>
       <c r="D31" s="1" t="s">
-        <v>62</v>
-      </c>
-      <c r="E31">
-        <v>138</v>
-      </c>
-      <c r="F31" s="1"/>
-      <c r="G31" s="1"/>
-      <c r="H31" s="1"/>
-      <c r="I31" s="1"/>
-    </row>
-    <row r="32" spans="1:9" x14ac:dyDescent="0.4">
+        <v>44</v>
+      </c>
+      <c r="E31" s="12">
+        <v>40</v>
+      </c>
+      <c r="F31">
+        <v>714</v>
+      </c>
+      <c r="G31" s="1">
+        <v>1</v>
+      </c>
+      <c r="H31" s="1">
+        <v>1</v>
+      </c>
+      <c r="I31" s="1">
+        <v>0</v>
+      </c>
+      <c r="J31" s="1"/>
+    </row>
+    <row r="32" spans="1:10" x14ac:dyDescent="0.4">
       <c r="A32" s="3" t="s">
-        <v>63</v>
+        <v>45</v>
       </c>
       <c r="B32" s="1">
-        <v>10</v>
-      </c>
-      <c r="C32" s="1" t="s">
-        <v>135</v>
+        <v>56</v>
+      </c>
+      <c r="C32" s="1">
+        <v>24590</v>
       </c>
       <c r="D32" s="1" t="s">
-        <v>65</v>
-      </c>
-      <c r="E32">
-        <v>367</v>
-      </c>
-      <c r="F32" s="1"/>
-      <c r="G32" s="1">
-        <v>2</v>
-      </c>
-      <c r="H32" s="1">
-        <v>2</v>
-      </c>
+        <v>46</v>
+      </c>
+      <c r="E32" s="12">
+        <v>47</v>
+      </c>
+      <c r="F32">
+        <v>454</v>
+      </c>
+      <c r="G32" s="1"/>
+      <c r="H32" s="1"/>
       <c r="I32" s="1"/>
-    </row>
-    <row r="33" spans="1:9" x14ac:dyDescent="0.4">
-      <c r="A33" s="3" t="s">
-        <v>66</v>
-      </c>
-      <c r="B33" s="1">
+      <c r="J32" s="1"/>
+    </row>
+    <row r="33" spans="1:10" x14ac:dyDescent="0.4">
+      <c r="A33" t="s">
+        <v>170</v>
+      </c>
+      <c r="C33" t="s">
+        <v>231</v>
+      </c>
+      <c r="E33" s="12">
+        <v>41</v>
+      </c>
+      <c r="F33">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="34" spans="1:10" x14ac:dyDescent="0.4">
+      <c r="A34" s="3" t="s">
+        <v>51</v>
+      </c>
+      <c r="B34" s="1">
         <v>7</v>
       </c>
-      <c r="C33" s="1" t="s">
-        <v>136</v>
-      </c>
-      <c r="D33" s="1" t="s">
-        <v>68</v>
-      </c>
-      <c r="E33">
-        <v>352</v>
-      </c>
-      <c r="F33" s="1"/>
-      <c r="G33" s="1">
-        <v>2</v>
-      </c>
-      <c r="H33" s="1">
-        <v>2</v>
-      </c>
-      <c r="I33" s="1"/>
-    </row>
-    <row r="34" spans="1:9" x14ac:dyDescent="0.4">
-      <c r="A34" s="6" t="s">
-        <v>78</v>
-      </c>
-      <c r="B34" s="1">
+      <c r="C34" s="1" t="s">
+        <v>131</v>
+      </c>
+      <c r="D34" s="1" t="s">
+        <v>53</v>
+      </c>
+      <c r="E34" s="12">
+        <v>69</v>
+      </c>
+      <c r="F34">
+        <v>199</v>
+      </c>
+      <c r="G34" s="1"/>
+      <c r="H34" s="1">
+        <v>4</v>
+      </c>
+      <c r="I34" s="1">
+        <v>4</v>
+      </c>
+      <c r="J34" s="1"/>
+    </row>
+    <row r="35" spans="1:10" x14ac:dyDescent="0.4">
+      <c r="A35" s="3" t="s">
+        <v>54</v>
+      </c>
+      <c r="B35" s="1">
         <v>6</v>
       </c>
-      <c r="C34" s="1" t="s">
-        <v>137</v>
-      </c>
-      <c r="D34" s="1" t="s">
-        <v>69</v>
-      </c>
-      <c r="E34">
-        <v>412</v>
-      </c>
-      <c r="F34" s="1"/>
-      <c r="G34" s="1"/>
-      <c r="H34" s="1"/>
-      <c r="I34" s="1"/>
-    </row>
-    <row r="35" spans="1:9" x14ac:dyDescent="0.4">
-      <c r="A35" s="6" t="s">
+      <c r="C35" s="1" t="s">
+        <v>132</v>
+      </c>
+      <c r="D35" s="1" t="s">
+        <v>55</v>
+      </c>
+      <c r="E35" s="12">
         <v>70</v>
       </c>
-      <c r="B35" s="1">
-        <v>12</v>
-      </c>
-      <c r="C35" s="1" t="s">
-        <v>138</v>
-      </c>
-      <c r="D35" s="1" t="s">
-        <v>72</v>
-      </c>
-      <c r="E35">
-        <v>352</v>
-      </c>
-      <c r="F35" s="1"/>
-      <c r="G35" s="1">
-        <v>2</v>
-      </c>
+      <c r="F35">
+        <v>224</v>
+      </c>
+      <c r="G35" s="1"/>
       <c r="H35" s="1">
-        <v>2</v>
-      </c>
-      <c r="I35" s="1"/>
-    </row>
-    <row r="36" spans="1:9" x14ac:dyDescent="0.4">
-      <c r="A36" s="6" t="s">
-        <v>79</v>
-      </c>
-      <c r="B36" s="1">
+        <v>1</v>
+      </c>
+      <c r="I35" s="1">
+        <v>0</v>
+      </c>
+      <c r="J35" s="1"/>
+    </row>
+    <row r="36" spans="1:10" x14ac:dyDescent="0.4">
+      <c r="A36" t="s">
+        <v>232</v>
+      </c>
+      <c r="C36" t="s">
+        <v>201</v>
+      </c>
+      <c r="D36" s="10">
+        <v>45553</v>
+      </c>
+      <c r="E36" s="12">
+        <v>29</v>
+      </c>
+      <c r="F36">
+        <v>173</v>
+      </c>
+    </row>
+    <row r="37" spans="1:10" x14ac:dyDescent="0.4">
+      <c r="A37" s="3" t="s">
+        <v>56</v>
+      </c>
+      <c r="B37" s="1">
         <v>5</v>
       </c>
-      <c r="C36" s="1" t="s">
-        <v>139</v>
-      </c>
-      <c r="D36" s="1" t="s">
-        <v>73</v>
-      </c>
-      <c r="E36">
-        <v>42</v>
-      </c>
-      <c r="F36" s="1"/>
-      <c r="G36" s="1"/>
-      <c r="H36" s="1"/>
-      <c r="I36" s="1"/>
-    </row>
-    <row r="37" spans="1:9" x14ac:dyDescent="0.4">
-      <c r="A37" s="6" t="s">
-        <v>74</v>
-      </c>
-      <c r="B37" s="1">
-        <v>7</v>
-      </c>
       <c r="C37" s="1" t="s">
-        <v>140</v>
+        <v>133</v>
       </c>
       <c r="D37" s="1" t="s">
-        <v>76</v>
-      </c>
-      <c r="E37">
-        <v>25</v>
-      </c>
-      <c r="F37" s="1"/>
+        <v>57</v>
+      </c>
+      <c r="E37" s="12">
+        <v>31</v>
+      </c>
+      <c r="F37">
+        <v>31</v>
+      </c>
       <c r="G37" s="1"/>
       <c r="H37" s="1"/>
       <c r="I37" s="1"/>
-    </row>
-    <row r="38" spans="1:9" x14ac:dyDescent="0.4">
+      <c r="J37" s="1"/>
+    </row>
+    <row r="38" spans="1:10" x14ac:dyDescent="0.4">
       <c r="A38" t="s">
+        <v>169</v>
+      </c>
+      <c r="C38" t="s">
+        <v>203</v>
+      </c>
+      <c r="D38" s="10">
+        <v>45709</v>
+      </c>
+      <c r="E38" s="12">
+        <v>19</v>
+      </c>
+      <c r="F38">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="39" spans="1:10" x14ac:dyDescent="0.4">
+      <c r="A39" s="3" t="s">
+        <v>60</v>
+      </c>
+      <c r="B39" s="1">
+        <v>121</v>
+      </c>
+      <c r="C39" s="1" t="s">
+        <v>134</v>
+      </c>
+      <c r="D39" s="1" t="s">
+        <v>62</v>
+      </c>
+      <c r="E39" s="12">
+        <v>6</v>
+      </c>
+      <c r="F39">
+        <v>138</v>
+      </c>
+      <c r="G39" s="1"/>
+      <c r="H39" s="1"/>
+      <c r="I39" s="1"/>
+      <c r="J39" s="1"/>
+    </row>
+    <row r="40" spans="1:10" x14ac:dyDescent="0.4">
+      <c r="A40" s="3" t="s">
+        <v>63</v>
+      </c>
+      <c r="B40" s="1">
+        <v>10</v>
+      </c>
+      <c r="C40" s="1" t="s">
+        <v>135</v>
+      </c>
+      <c r="D40" s="1" t="s">
+        <v>65</v>
+      </c>
+      <c r="E40" s="12">
+        <v>41</v>
+      </c>
+      <c r="F40">
+        <v>367</v>
+      </c>
+      <c r="G40" s="1"/>
+      <c r="H40" s="1">
+        <v>2</v>
+      </c>
+      <c r="I40" s="1">
+        <v>2</v>
+      </c>
+      <c r="J40" s="1"/>
+    </row>
+    <row r="41" spans="1:10" x14ac:dyDescent="0.4">
+      <c r="A41" s="3" t="s">
+        <v>66</v>
+      </c>
+      <c r="B41" s="1">
+        <v>7</v>
+      </c>
+      <c r="C41" s="1" t="s">
+        <v>136</v>
+      </c>
+      <c r="D41" s="1" t="s">
+        <v>68</v>
+      </c>
+      <c r="E41" s="12">
+        <v>26</v>
+      </c>
+      <c r="F41">
+        <v>352</v>
+      </c>
+      <c r="G41" s="1"/>
+      <c r="H41" s="1">
+        <v>2</v>
+      </c>
+      <c r="I41" s="1">
+        <v>2</v>
+      </c>
+      <c r="J41" s="1"/>
+    </row>
+    <row r="42" spans="1:10" x14ac:dyDescent="0.4">
+      <c r="A42" s="6" t="s">
+        <v>78</v>
+      </c>
+      <c r="B42" s="1">
+        <v>6</v>
+      </c>
+      <c r="C42" s="1" t="s">
+        <v>137</v>
+      </c>
+      <c r="D42" s="1" t="s">
+        <v>69</v>
+      </c>
+      <c r="E42" s="12">
+        <v>29</v>
+      </c>
+      <c r="F42">
+        <v>412</v>
+      </c>
+      <c r="G42" s="1"/>
+      <c r="H42" s="1"/>
+      <c r="I42" s="1"/>
+      <c r="J42" s="1"/>
+    </row>
+    <row r="43" spans="1:10" x14ac:dyDescent="0.4">
+      <c r="A43" s="6" t="s">
+        <v>70</v>
+      </c>
+      <c r="B43" s="1">
+        <v>12</v>
+      </c>
+      <c r="C43" s="1" t="s">
+        <v>138</v>
+      </c>
+      <c r="D43" s="1" t="s">
+        <v>72</v>
+      </c>
+      <c r="E43" s="12">
+        <v>68</v>
+      </c>
+      <c r="F43">
+        <v>352</v>
+      </c>
+      <c r="G43" s="1"/>
+      <c r="H43" s="1">
+        <v>2</v>
+      </c>
+      <c r="I43" s="1">
+        <v>2</v>
+      </c>
+      <c r="J43" s="1"/>
+    </row>
+    <row r="44" spans="1:10" x14ac:dyDescent="0.4">
+      <c r="A44" s="6" t="s">
+        <v>79</v>
+      </c>
+      <c r="B44" s="1">
+        <v>5</v>
+      </c>
+      <c r="C44" s="1" t="s">
+        <v>139</v>
+      </c>
+      <c r="D44" s="1" t="s">
+        <v>73</v>
+      </c>
+      <c r="E44" s="12">
+        <v>6</v>
+      </c>
+      <c r="F44">
+        <v>42</v>
+      </c>
+      <c r="G44" s="1"/>
+      <c r="H44" s="1"/>
+      <c r="I44" s="1"/>
+      <c r="J44" s="1"/>
+    </row>
+    <row r="45" spans="1:10" x14ac:dyDescent="0.4">
+      <c r="A45" s="6" t="s">
+        <v>74</v>
+      </c>
+      <c r="B45" s="1">
+        <v>7</v>
+      </c>
+      <c r="C45" s="1" t="s">
+        <v>140</v>
+      </c>
+      <c r="D45" s="1" t="s">
+        <v>76</v>
+      </c>
+      <c r="E45" s="12">
+        <v>30</v>
+      </c>
+      <c r="F45">
+        <v>25</v>
+      </c>
+      <c r="G45" s="1"/>
+      <c r="H45" s="1"/>
+      <c r="I45" s="1"/>
+      <c r="J45" s="1"/>
+    </row>
+    <row r="46" spans="1:10" x14ac:dyDescent="0.4">
+      <c r="A46" t="s">
         <v>146</v>
       </c>
-      <c r="B38" t="s">
+      <c r="B46" t="s">
         <v>147</v>
       </c>
-      <c r="C38" s="1" t="s">
+      <c r="C46" s="1" t="s">
         <v>197</v>
       </c>
-      <c r="D38" s="10">
+      <c r="D46" s="10">
         <v>41564</v>
       </c>
-      <c r="E38">
+      <c r="F46">
         <v>4162</v>
       </c>
-      <c r="F38">
-        <v>2</v>
-      </c>
-      <c r="G38">
+      <c r="G46">
+        <v>2</v>
+      </c>
+      <c r="H46">
         <v>13</v>
       </c>
-      <c r="H38">
+      <c r="I46">
         <v>11</v>
       </c>
     </row>
-    <row r="39" spans="1:9" x14ac:dyDescent="0.4">
-      <c r="A39" t="s">
+    <row r="47" spans="1:10" x14ac:dyDescent="0.4">
+      <c r="A47" t="s">
         <v>149</v>
       </c>
-      <c r="C39" s="1" t="s">
+      <c r="C47" s="1" t="s">
         <v>198</v>
       </c>
-      <c r="D39" s="10">
+      <c r="D47" s="10">
         <v>41619</v>
       </c>
-      <c r="E39" s="1">
+      <c r="F47" s="1">
         <v>4107</v>
       </c>
-      <c r="F39">
+      <c r="G47">
         <v>3</v>
       </c>
-      <c r="G39">
+      <c r="H47">
         <v>3</v>
       </c>
-      <c r="H39">
+      <c r="I47">
         <v>0</v>
       </c>
     </row>
-    <row r="40" spans="1:9" x14ac:dyDescent="0.4">
-      <c r="A40" t="s">
+    <row r="48" spans="1:10" x14ac:dyDescent="0.4">
+      <c r="A48" t="s">
         <v>150</v>
       </c>
-      <c r="C40" t="s">
+      <c r="C48" t="s">
         <v>198</v>
       </c>
-      <c r="D40" s="10">
+      <c r="D48" s="10">
         <v>41619</v>
       </c>
-      <c r="E40" s="1">
+      <c r="E48" s="12">
+        <v>6</v>
+      </c>
+      <c r="F48" s="1">
         <v>4107</v>
       </c>
-      <c r="F40">
-        <v>2</v>
-      </c>
-      <c r="G40">
-        <v>2</v>
-      </c>
-      <c r="H40">
+      <c r="G48">
+        <v>2</v>
+      </c>
+      <c r="H48">
+        <v>2</v>
+      </c>
+      <c r="I48">
         <v>0</v>
       </c>
     </row>
-    <row r="41" spans="1:9" x14ac:dyDescent="0.4">
-      <c r="A41" t="s">
+    <row r="49" spans="1:9" x14ac:dyDescent="0.4">
+      <c r="A49" t="s">
         <v>151</v>
       </c>
-      <c r="C41" s="1" t="s">
+      <c r="C49" s="1" t="s">
         <v>198</v>
       </c>
-      <c r="D41" s="10">
+      <c r="D49" s="10">
         <v>41619</v>
       </c>
-      <c r="E41" s="1">
+      <c r="F49" s="1">
         <v>4107</v>
       </c>
-      <c r="F41">
-        <v>2</v>
-      </c>
-      <c r="G41">
-        <v>2</v>
-      </c>
-      <c r="H41">
+      <c r="G49">
+        <v>2</v>
+      </c>
+      <c r="H49">
+        <v>2</v>
+      </c>
+      <c r="I49">
         <v>0</v>
       </c>
     </row>
-    <row r="42" spans="1:9" x14ac:dyDescent="0.4">
-      <c r="A42" t="s">
+    <row r="50" spans="1:9" x14ac:dyDescent="0.4">
+      <c r="A50" t="s">
         <v>152</v>
-      </c>
-      <c r="C42" t="s">
-        <v>199</v>
-      </c>
-      <c r="D42" s="10">
-        <v>39092</v>
-      </c>
-      <c r="E42" s="1">
-        <v>6634</v>
-      </c>
-      <c r="F42">
-        <v>2</v>
-      </c>
-      <c r="G42">
-        <v>3</v>
-      </c>
-      <c r="H42">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="43" spans="1:9" x14ac:dyDescent="0.4">
-      <c r="A43" t="s">
-        <v>153</v>
-      </c>
-      <c r="C43" t="s">
-        <v>199</v>
-      </c>
-      <c r="D43" s="10">
-        <v>39092</v>
-      </c>
-      <c r="E43">
-        <v>6634</v>
-      </c>
-      <c r="F43">
-        <v>2</v>
-      </c>
-      <c r="G43">
-        <v>2</v>
-      </c>
-      <c r="H43">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="44" spans="1:9" x14ac:dyDescent="0.4">
-      <c r="A44" t="s">
-        <v>154</v>
-      </c>
-      <c r="C44" t="s">
-        <v>199</v>
-      </c>
-      <c r="D44" s="10">
-        <v>39092</v>
-      </c>
-      <c r="E44">
-        <v>6634</v>
-      </c>
-      <c r="F44">
-        <v>2</v>
-      </c>
-      <c r="G44">
-        <v>2</v>
-      </c>
-      <c r="H44">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="45" spans="1:9" x14ac:dyDescent="0.4">
-      <c r="A45" t="s">
-        <v>155</v>
-      </c>
-      <c r="C45" t="s">
-        <v>199</v>
-      </c>
-      <c r="D45" s="10">
-        <v>39092</v>
-      </c>
-      <c r="E45">
-        <v>6634</v>
-      </c>
-      <c r="F45">
-        <v>2</v>
-      </c>
-      <c r="G45">
-        <v>2</v>
-      </c>
-      <c r="H45">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="46" spans="1:9" x14ac:dyDescent="0.4">
-      <c r="A46" t="s">
-        <v>156</v>
-      </c>
-      <c r="C46" t="s">
-        <v>199</v>
-      </c>
-      <c r="D46" s="10">
-        <v>39092</v>
-      </c>
-      <c r="E46">
-        <v>6634</v>
-      </c>
-      <c r="F46">
-        <v>2</v>
-      </c>
-      <c r="G46">
-        <v>2</v>
-      </c>
-      <c r="H46">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="47" spans="1:9" x14ac:dyDescent="0.4">
-      <c r="A47" t="s">
-        <v>157</v>
-      </c>
-      <c r="C47" t="s">
-        <v>199</v>
-      </c>
-      <c r="D47" s="10">
-        <v>39092</v>
-      </c>
-      <c r="E47">
-        <v>6634</v>
-      </c>
-      <c r="F47">
-        <v>2</v>
-      </c>
-      <c r="G47">
-        <v>2</v>
-      </c>
-      <c r="H47">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="48" spans="1:9" x14ac:dyDescent="0.4">
-      <c r="A48" t="s">
-        <v>158</v>
-      </c>
-      <c r="C48" t="s">
-        <v>199</v>
-      </c>
-      <c r="D48" s="10">
-        <v>39092</v>
-      </c>
-      <c r="E48">
-        <v>6634</v>
-      </c>
-      <c r="F48">
-        <v>2</v>
-      </c>
-      <c r="G48">
-        <v>2</v>
-      </c>
-      <c r="H48">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="49" spans="1:8" x14ac:dyDescent="0.4">
-      <c r="A49" t="s">
-        <v>159</v>
-      </c>
-      <c r="C49" t="s">
-        <v>199</v>
-      </c>
-      <c r="D49" s="10">
-        <v>39092</v>
-      </c>
-      <c r="E49">
-        <v>6634</v>
-      </c>
-      <c r="F49">
-        <v>2</v>
-      </c>
-      <c r="G49">
-        <v>2</v>
-      </c>
-      <c r="H49">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="50" spans="1:8" x14ac:dyDescent="0.4">
-      <c r="A50" t="s">
-        <v>160</v>
       </c>
       <c r="C50" t="s">
         <v>199</v>
@@ -2317,20 +2375,20 @@
       <c r="D50" s="10">
         <v>39092</v>
       </c>
-      <c r="E50">
+      <c r="F50" s="1">
         <v>6634</v>
       </c>
-      <c r="F50">
-        <v>2</v>
-      </c>
       <c r="G50">
         <v>2</v>
       </c>
       <c r="H50">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="51" spans="1:8" x14ac:dyDescent="0.4">
+        <v>3</v>
+      </c>
+      <c r="I50">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="51" spans="1:9" x14ac:dyDescent="0.4">
       <c r="A51" t="s">
         <v>161</v>
       </c>
@@ -2340,20 +2398,20 @@
       <c r="D51" s="10">
         <v>39092</v>
       </c>
-      <c r="E51">
+      <c r="F51">
         <v>6634</v>
       </c>
-      <c r="F51">
-        <v>2</v>
-      </c>
       <c r="G51">
         <v>2</v>
       </c>
       <c r="H51">
+        <v>2</v>
+      </c>
+      <c r="I51">
         <v>0</v>
       </c>
     </row>
-    <row r="52" spans="1:8" x14ac:dyDescent="0.4">
+    <row r="52" spans="1:9" x14ac:dyDescent="0.4">
       <c r="A52" t="s">
         <v>162</v>
       </c>
@@ -2363,20 +2421,20 @@
       <c r="D52" s="10">
         <v>39092</v>
       </c>
-      <c r="E52">
+      <c r="F52">
         <v>6634</v>
       </c>
-      <c r="F52">
-        <v>2</v>
-      </c>
       <c r="G52">
         <v>2</v>
       </c>
       <c r="H52">
+        <v>2</v>
+      </c>
+      <c r="I52">
         <v>0</v>
       </c>
     </row>
-    <row r="53" spans="1:8" x14ac:dyDescent="0.4">
+    <row r="53" spans="1:9" x14ac:dyDescent="0.4">
       <c r="A53" t="s">
         <v>163</v>
       </c>
@@ -2386,20 +2444,20 @@
       <c r="D53" s="10">
         <v>39092</v>
       </c>
-      <c r="E53">
+      <c r="F53">
         <v>6634</v>
       </c>
-      <c r="F53">
-        <v>2</v>
-      </c>
       <c r="G53">
         <v>2</v>
       </c>
       <c r="H53">
+        <v>2</v>
+      </c>
+      <c r="I53">
         <v>0</v>
       </c>
     </row>
-    <row r="54" spans="1:8" x14ac:dyDescent="0.4">
+    <row r="54" spans="1:9" x14ac:dyDescent="0.4">
       <c r="A54" t="s">
         <v>164</v>
       </c>
@@ -2409,209 +2467,293 @@
       <c r="D54" s="10">
         <v>39092</v>
       </c>
-      <c r="E54">
+      <c r="F54">
         <v>6634</v>
       </c>
-      <c r="F54">
-        <v>2</v>
-      </c>
       <c r="G54">
         <v>2</v>
       </c>
       <c r="H54">
+        <v>2</v>
+      </c>
+      <c r="I54">
         <v>0</v>
       </c>
     </row>
-    <row r="55" spans="1:8" x14ac:dyDescent="0.4">
+    <row r="55" spans="1:9" x14ac:dyDescent="0.4">
       <c r="A55" t="s">
+        <v>153</v>
+      </c>
+      <c r="C55" t="s">
+        <v>199</v>
+      </c>
+      <c r="D55" s="10">
+        <v>39092</v>
+      </c>
+      <c r="F55">
+        <v>6634</v>
+      </c>
+      <c r="G55">
+        <v>2</v>
+      </c>
+      <c r="H55">
+        <v>2</v>
+      </c>
+      <c r="I55">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="56" spans="1:9" x14ac:dyDescent="0.4">
+      <c r="A56" t="s">
+        <v>154</v>
+      </c>
+      <c r="C56" t="s">
+        <v>199</v>
+      </c>
+      <c r="D56" s="10">
+        <v>39092</v>
+      </c>
+      <c r="F56">
+        <v>6634</v>
+      </c>
+      <c r="G56">
+        <v>2</v>
+      </c>
+      <c r="H56">
+        <v>2</v>
+      </c>
+      <c r="I56">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="57" spans="1:9" x14ac:dyDescent="0.4">
+      <c r="A57" t="s">
+        <v>155</v>
+      </c>
+      <c r="C57" t="s">
+        <v>199</v>
+      </c>
+      <c r="D57" s="10">
+        <v>39092</v>
+      </c>
+      <c r="F57">
+        <v>6634</v>
+      </c>
+      <c r="G57">
+        <v>2</v>
+      </c>
+      <c r="H57">
+        <v>2</v>
+      </c>
+      <c r="I57">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="58" spans="1:9" x14ac:dyDescent="0.4">
+      <c r="A58" t="s">
+        <v>156</v>
+      </c>
+      <c r="C58" t="s">
+        <v>199</v>
+      </c>
+      <c r="D58" s="10">
+        <v>39092</v>
+      </c>
+      <c r="F58">
+        <v>6634</v>
+      </c>
+      <c r="G58">
+        <v>2</v>
+      </c>
+      <c r="H58">
+        <v>2</v>
+      </c>
+      <c r="I58">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="59" spans="1:9" x14ac:dyDescent="0.4">
+      <c r="A59" t="s">
+        <v>157</v>
+      </c>
+      <c r="C59" t="s">
+        <v>199</v>
+      </c>
+      <c r="D59" s="10">
+        <v>39092</v>
+      </c>
+      <c r="F59">
+        <v>6634</v>
+      </c>
+      <c r="G59">
+        <v>2</v>
+      </c>
+      <c r="H59">
+        <v>2</v>
+      </c>
+      <c r="I59">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="60" spans="1:9" x14ac:dyDescent="0.4">
+      <c r="A60" t="s">
+        <v>158</v>
+      </c>
+      <c r="C60" t="s">
+        <v>199</v>
+      </c>
+      <c r="D60" s="10">
+        <v>39092</v>
+      </c>
+      <c r="F60">
+        <v>6634</v>
+      </c>
+      <c r="G60">
+        <v>2</v>
+      </c>
+      <c r="H60">
+        <v>2</v>
+      </c>
+      <c r="I60">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="61" spans="1:9" x14ac:dyDescent="0.4">
+      <c r="A61" t="s">
+        <v>159</v>
+      </c>
+      <c r="C61" t="s">
+        <v>199</v>
+      </c>
+      <c r="D61" s="10">
+        <v>39092</v>
+      </c>
+      <c r="F61">
+        <v>6634</v>
+      </c>
+      <c r="G61">
+        <v>2</v>
+      </c>
+      <c r="H61">
+        <v>2</v>
+      </c>
+      <c r="I61">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="62" spans="1:9" x14ac:dyDescent="0.4">
+      <c r="A62" t="s">
+        <v>160</v>
+      </c>
+      <c r="C62" t="s">
+        <v>199</v>
+      </c>
+      <c r="D62" s="10">
+        <v>39092</v>
+      </c>
+      <c r="F62">
+        <v>6634</v>
+      </c>
+      <c r="G62">
+        <v>2</v>
+      </c>
+      <c r="H62">
+        <v>2</v>
+      </c>
+      <c r="I62">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="63" spans="1:9" x14ac:dyDescent="0.4">
+      <c r="A63" t="s">
         <v>165</v>
       </c>
-      <c r="C55" t="s">
+      <c r="C63" t="s">
         <v>200</v>
       </c>
-      <c r="D55" s="10">
+      <c r="D63" s="10">
         <v>42975</v>
       </c>
-      <c r="E55">
+      <c r="F63">
         <v>2571</v>
       </c>
-      <c r="F55">
+      <c r="G63">
         <v>0</v>
       </c>
-      <c r="G55">
+      <c r="H63">
         <v>1</v>
       </c>
-      <c r="H55">
+      <c r="I63">
         <v>1</v>
       </c>
     </row>
-    <row r="56" spans="1:8" x14ac:dyDescent="0.4">
-      <c r="A56" t="s">
-        <v>169</v>
-      </c>
-      <c r="C56" t="s">
-        <v>203</v>
-      </c>
-      <c r="D56" s="10">
-        <v>45709</v>
-      </c>
-      <c r="E56">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="57" spans="1:8" x14ac:dyDescent="0.4">
-      <c r="A57" t="s">
-        <v>232</v>
-      </c>
-      <c r="C57" t="s">
-        <v>201</v>
-      </c>
-      <c r="D57" s="10">
-        <v>45553</v>
-      </c>
-      <c r="E57">
-        <v>173</v>
-      </c>
-    </row>
-    <row r="58" spans="1:8" x14ac:dyDescent="0.4">
-      <c r="A58" t="s">
-        <v>226</v>
-      </c>
-      <c r="C58" t="s">
-        <v>202</v>
-      </c>
-      <c r="D58" s="10">
-        <v>45069</v>
-      </c>
-      <c r="E58">
-        <v>657</v>
-      </c>
-    </row>
-    <row r="59" spans="1:8" x14ac:dyDescent="0.4">
-      <c r="A59" t="s">
-        <v>227</v>
-      </c>
-      <c r="C59" t="s">
-        <v>204</v>
-      </c>
-      <c r="D59" s="10">
-        <v>44928</v>
-      </c>
-      <c r="E59">
-        <v>798</v>
-      </c>
-    </row>
-    <row r="60" spans="1:8" x14ac:dyDescent="0.4">
-      <c r="A60" t="s">
-        <v>228</v>
-      </c>
-      <c r="C60" t="s">
-        <v>205</v>
-      </c>
-      <c r="D60" s="10">
-        <v>44812</v>
-      </c>
-      <c r="E60">
-        <v>914</v>
-      </c>
-    </row>
-    <row r="61" spans="1:8" x14ac:dyDescent="0.4">
-      <c r="A61" t="s">
-        <v>229</v>
-      </c>
-      <c r="C61" t="s">
-        <v>209</v>
-      </c>
-      <c r="D61" s="10">
-        <v>44371</v>
-      </c>
-      <c r="E61">
-        <v>1355</v>
-      </c>
-    </row>
-    <row r="62" spans="1:8" x14ac:dyDescent="0.4">
-      <c r="A62" t="s">
+    <row r="64" spans="1:9" x14ac:dyDescent="0.4">
+      <c r="A64" t="s">
         <v>176</v>
       </c>
-      <c r="C62" t="s">
+      <c r="C64" t="s">
         <v>208</v>
       </c>
-      <c r="D62" s="10">
+      <c r="D64" s="10">
         <v>44294</v>
       </c>
-      <c r="E62">
+      <c r="E64" s="13">
+        <v>57</v>
+      </c>
+      <c r="F64">
         <v>1432</v>
       </c>
     </row>
-    <row r="63" spans="1:8" x14ac:dyDescent="0.4">
-      <c r="A63" t="s">
-        <v>230</v>
-      </c>
-      <c r="C63" t="s">
-        <v>206</v>
-      </c>
-      <c r="D63" s="10">
-        <v>44067</v>
-      </c>
-      <c r="E63">
-        <v>1294</v>
-      </c>
-    </row>
-    <row r="64" spans="1:8" x14ac:dyDescent="0.4">
-      <c r="A64" t="s">
+    <row r="65" spans="1:6" x14ac:dyDescent="0.4">
+      <c r="A65" t="s">
         <v>178</v>
       </c>
-      <c r="C64" t="s">
+      <c r="C65" t="s">
         <v>207</v>
       </c>
-      <c r="D64" s="10">
+      <c r="D65" s="10">
         <v>44013</v>
       </c>
-      <c r="E64">
+      <c r="E65" s="13">
+        <v>26</v>
+      </c>
+      <c r="F65">
         <v>1348</v>
       </c>
     </row>
-    <row r="65" spans="1:5" x14ac:dyDescent="0.4">
-      <c r="A65" t="s">
-        <v>170</v>
-      </c>
-      <c r="C65" t="s">
-        <v>231</v>
-      </c>
-      <c r="E65">
-        <v>53</v>
-      </c>
-    </row>
   </sheetData>
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A5:J65">
+    <sortCondition ref="A5:A65"/>
+  </sortState>
   <hyperlinks>
-    <hyperlink ref="A6" r:id="rId1" location="2020-178" display="https://s3-internal.ki.se/ui/ - 2020-178" xr:uid="{4704F72A-9F53-4D00-A05B-C45AE37FBFAF}"/>
-    <hyperlink ref="A7" r:id="rId2" location="2021-108" display="https://s3-internal.ki.se/ui/ - 2021-108" xr:uid="{07F6BC8D-A4BB-47E7-B480-CBB1D14CF27B}"/>
-    <hyperlink ref="A9" r:id="rId3" location="2021-310" display="https://s3-internal.ki.se/ui/ - 2021-310" xr:uid="{AB1E1F0C-C690-45CD-B2AA-5FC8034D146D}"/>
-    <hyperlink ref="A10" r:id="rId4" location="2021-311" display="https://s3-internal.ki.se/ui/ - 2021-311" xr:uid="{4C930C7F-636A-4B4F-9412-55F7E7FF41BE}"/>
-    <hyperlink ref="A11" r:id="rId5" location="2021-331" display="https://s3-internal.ki.se/ui/ - 2021-331" xr:uid="{02097C05-ADE1-41F6-9F7E-3E80B573FDA8}"/>
-    <hyperlink ref="A12" r:id="rId6" location="2021-340" display="https://s3-internal.ki.se/ui/ - 2021-340" xr:uid="{DFE18941-59B4-4A23-B1AB-144354BB2D3B}"/>
-    <hyperlink ref="A13" r:id="rId7" location="2021-68" display="https://s3-internal.ki.se/ui/ - 2021-68" xr:uid="{6D1FC617-382C-4E19-B823-A63D6084B94D}"/>
-    <hyperlink ref="A14" r:id="rId8" location="2022-113" display="https://s3-internal.ki.se/ui/ - 2022-113" xr:uid="{3223DB82-EF69-40C2-9B35-AE19F917DB59}"/>
-    <hyperlink ref="A15" r:id="rId9" location="2023-106" display="https://s3-internal.ki.se/ui/ - 2023-106" xr:uid="{1174C04C-DB1E-4BA3-872D-DA0C7942FE46}"/>
-    <hyperlink ref="A16" r:id="rId10" location="2023-118" display="https://s3-internal.ki.se/ui/ - 2023-118" xr:uid="{715BCA2F-430F-413B-8397-FE44920AF35A}"/>
-    <hyperlink ref="A17" r:id="rId11" location="2023-120" display="https://s3-internal.ki.se/ui/ - 2023-120" xr:uid="{7FE5FEAC-B1AE-407A-948A-1E7037024B7B}"/>
-    <hyperlink ref="A18" r:id="rId12" location="2023-121" display="https://s3-internal.ki.se/ui/ - 2023-121" xr:uid="{5877598B-3677-42EF-AD76-CCE2D107431B}"/>
-    <hyperlink ref="A19" r:id="rId13" location="2023-122" display="https://s3-internal.ki.se/ui/ - 2023-122" xr:uid="{AC763F6E-36B0-4706-8062-E5FCAC3FAFD0}"/>
-    <hyperlink ref="A20" r:id="rId14" location="2023-148" display="https://s3-internal.ki.se/ui/ - 2023-148" xr:uid="{3DAD76BE-C4EC-4B6B-8060-3A7CD54FD4D4}"/>
-    <hyperlink ref="A21" r:id="rId15" location="2023-183" display="https://s3-internal.ki.se/ui/ - 2023-183" xr:uid="{BB096BD3-CFCB-40A3-B141-BA592810E168}"/>
-    <hyperlink ref="A22" r:id="rId16" location="2023-217" display="https://s3-internal.ki.se/ui/ - 2023-217" xr:uid="{01CDE55F-17EA-427A-B2AF-F5793C8413A8}"/>
-    <hyperlink ref="A23" r:id="rId17" location="2023-222" display="https://s3-internal.ki.se/ui/ - 2023-222" xr:uid="{879DC4A6-D604-4CF8-871E-122F7852313F}"/>
-    <hyperlink ref="A24" r:id="rId18" location="2023-223" display="https://s3-internal.ki.se/ui/ - 2023-223" xr:uid="{D364C9D6-0179-47C3-A0C0-F15C37CC5403}"/>
-    <hyperlink ref="A25" r:id="rId19" location="2023-227" display="https://s3-internal.ki.se/ui/ - 2023-227" xr:uid="{678CFFD7-8C72-4A48-98FA-3AC0FDE6737F}"/>
-    <hyperlink ref="A26" r:id="rId20" location="2023-28" display="https://s3-internal.ki.se/ui/ - 2023-28" xr:uid="{6D75B920-1E4B-424E-8E4D-4804B8C9E0EC}"/>
-    <hyperlink ref="A27" r:id="rId21" location="2023-289" display="https://s3-internal.ki.se/ui/ - 2023-289" xr:uid="{18D5751C-9C9B-4B40-AFDD-12234AF2B23F}"/>
-    <hyperlink ref="A28" r:id="rId22" location="2024-438" display="https://s3-internal.ki.se/ui/ - 2024-438" xr:uid="{6F7B37CE-8C77-4B39-A6DF-8AB9A9C99EAC}"/>
-    <hyperlink ref="A29" r:id="rId23" location="2024-444" display="https://s3-internal.ki.se/ui/ - 2024-444" xr:uid="{B4A6F838-6C01-465F-ABFF-13220CA284E9}"/>
-    <hyperlink ref="A30" r:id="rId24" location="2024-486" display="https://s3-internal.ki.se/ui/ - 2024-486" xr:uid="{CC86EA3C-92E6-4B99-89FE-C2696FFE3FD4}"/>
-    <hyperlink ref="A31" r:id="rId25" location="2024-505" display="https://s3-internal.ki.se/ui/ - 2024-505" xr:uid="{4F54D22A-FCB4-4422-9895-E1396807069B}"/>
-    <hyperlink ref="A32" r:id="rId26" location="2024-78" display="https://s3-internal.ki.se/ui/ - 2024-78" xr:uid="{F0342A26-0688-4D86-A6BB-4942545684B1}"/>
-    <hyperlink ref="A33" r:id="rId27" location="2024-89" display="https://s3-internal.ki.se/ui/ - 2024-89" xr:uid="{BBC87D51-3B63-4A84-8C1E-4CEA3710A9F7}"/>
-    <hyperlink ref="A37" r:id="rId28" location="2025-21" display="https://s3-internal.ki.se/ui/ - 2025-21" xr:uid="{0E3B49EA-F46C-4CBD-B780-CD6D767CFE85}"/>
+    <hyperlink ref="A5" r:id="rId1" location="2020-178" display="https://s3-internal.ki.se/ui/ - 2020-178" xr:uid="{4704F72A-9F53-4D00-A05B-C45AE37FBFAF}"/>
+    <hyperlink ref="A9" r:id="rId2" location="2021-108" display="https://s3-internal.ki.se/ui/ - 2021-108" xr:uid="{07F6BC8D-A4BB-47E7-B480-CBB1D14CF27B}"/>
+    <hyperlink ref="A11" r:id="rId3" location="2021-310" display="https://s3-internal.ki.se/ui/ - 2021-310" xr:uid="{AB1E1F0C-C690-45CD-B2AA-5FC8034D146D}"/>
+    <hyperlink ref="A12" r:id="rId4" location="2021-311" display="https://s3-internal.ki.se/ui/ - 2021-311" xr:uid="{4C930C7F-636A-4B4F-9412-55F7E7FF41BE}"/>
+    <hyperlink ref="A13" r:id="rId5" location="2021-331" display="https://s3-internal.ki.se/ui/ - 2021-331" xr:uid="{02097C05-ADE1-41F6-9F7E-3E80B573FDA8}"/>
+    <hyperlink ref="A14" r:id="rId6" location="2021-340" display="https://s3-internal.ki.se/ui/ - 2021-340" xr:uid="{DFE18941-59B4-4A23-B1AB-144354BB2D3B}"/>
+    <hyperlink ref="A15" r:id="rId7" location="2021-68" display="https://s3-internal.ki.se/ui/ - 2021-68" xr:uid="{6D1FC617-382C-4E19-B823-A63D6084B94D}"/>
+    <hyperlink ref="A17" r:id="rId8" location="2022-113" display="https://s3-internal.ki.se/ui/ - 2022-113" xr:uid="{3223DB82-EF69-40C2-9B35-AE19F917DB59}"/>
+    <hyperlink ref="A19" r:id="rId9" location="2023-106" display="https://s3-internal.ki.se/ui/ - 2023-106" xr:uid="{1174C04C-DB1E-4BA3-872D-DA0C7942FE46}"/>
+    <hyperlink ref="A21" r:id="rId10" location="2023-118" display="https://s3-internal.ki.se/ui/ - 2023-118" xr:uid="{715BCA2F-430F-413B-8397-FE44920AF35A}"/>
+    <hyperlink ref="A22" r:id="rId11" location="2023-120" display="https://s3-internal.ki.se/ui/ - 2023-120" xr:uid="{7FE5FEAC-B1AE-407A-948A-1E7037024B7B}"/>
+    <hyperlink ref="A23" r:id="rId12" location="2023-121" display="https://s3-internal.ki.se/ui/ - 2023-121" xr:uid="{5877598B-3677-42EF-AD76-CCE2D107431B}"/>
+    <hyperlink ref="A24" r:id="rId13" location="2023-122" display="https://s3-internal.ki.se/ui/ - 2023-122" xr:uid="{AC763F6E-36B0-4706-8062-E5FCAC3FAFD0}"/>
+    <hyperlink ref="A25" r:id="rId14" location="2023-148" display="https://s3-internal.ki.se/ui/ - 2023-148" xr:uid="{3DAD76BE-C4EC-4B6B-8060-3A7CD54FD4D4}"/>
+    <hyperlink ref="A26" r:id="rId15" location="2023-183" display="https://s3-internal.ki.se/ui/ - 2023-183" xr:uid="{BB096BD3-CFCB-40A3-B141-BA592810E168}"/>
+    <hyperlink ref="A27" r:id="rId16" location="2023-217" display="https://s3-internal.ki.se/ui/ - 2023-217" xr:uid="{01CDE55F-17EA-427A-B2AF-F5793C8413A8}"/>
+    <hyperlink ref="A28" r:id="rId17" location="2023-222" display="https://s3-internal.ki.se/ui/ - 2023-222" xr:uid="{879DC4A6-D604-4CF8-871E-122F7852313F}"/>
+    <hyperlink ref="A29" r:id="rId18" location="2023-223" display="https://s3-internal.ki.se/ui/ - 2023-223" xr:uid="{D364C9D6-0179-47C3-A0C0-F15C37CC5403}"/>
+    <hyperlink ref="A30" r:id="rId19" location="2023-227" display="https://s3-internal.ki.se/ui/ - 2023-227" xr:uid="{678CFFD7-8C72-4A48-98FA-3AC0FDE6737F}"/>
+    <hyperlink ref="A31" r:id="rId20" location="2023-28" display="https://s3-internal.ki.se/ui/ - 2023-28" xr:uid="{6D75B920-1E4B-424E-8E4D-4804B8C9E0EC}"/>
+    <hyperlink ref="A32" r:id="rId21" location="2023-289" display="https://s3-internal.ki.se/ui/ - 2023-289" xr:uid="{18D5751C-9C9B-4B40-AFDD-12234AF2B23F}"/>
+    <hyperlink ref="A34" r:id="rId22" location="2024-438" display="https://s3-internal.ki.se/ui/ - 2024-438" xr:uid="{6F7B37CE-8C77-4B39-A6DF-8AB9A9C99EAC}"/>
+    <hyperlink ref="A35" r:id="rId23" location="2024-444" display="https://s3-internal.ki.se/ui/ - 2024-444" xr:uid="{B4A6F838-6C01-465F-ABFF-13220CA284E9}"/>
+    <hyperlink ref="A37" r:id="rId24" location="2024-486" display="https://s3-internal.ki.se/ui/ - 2024-486" xr:uid="{CC86EA3C-92E6-4B99-89FE-C2696FFE3FD4}"/>
+    <hyperlink ref="A39" r:id="rId25" location="2024-505" display="https://s3-internal.ki.se/ui/ - 2024-505" xr:uid="{4F54D22A-FCB4-4422-9895-E1396807069B}"/>
+    <hyperlink ref="A40" r:id="rId26" location="2024-78" display="https://s3-internal.ki.se/ui/ - 2024-78" xr:uid="{F0342A26-0688-4D86-A6BB-4942545684B1}"/>
+    <hyperlink ref="A41" r:id="rId27" location="2024-89" display="https://s3-internal.ki.se/ui/ - 2024-89" xr:uid="{BBC87D51-3B63-4A84-8C1E-4CEA3710A9F7}"/>
+    <hyperlink ref="A45" r:id="rId28" location="2025-21" display="https://s3-internal.ki.se/ui/ - 2025-21" xr:uid="{0E3B49EA-F46C-4CBD-B780-CD6D767CFE85}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId29"/>

</xml_diff>